<commit_message>
skill info table - category - 넘버링 변경
</commit_message>
<xml_diff>
--- a/로스트아크/데이터테이블/Skill_Info_Table(수정필요).xlsx
+++ b/로스트아크/데이터테이블/Skill_Info_Table(수정필요).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sky20\Desktop\진선\GameDesign\로스트아크\데이터테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6C97CFA-A756-4E80-BDCA-4CDB532748D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B007FF-3662-4E23-9637-2595D65377A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8E3DD992-F5CA-43CA-A90A-D3D2390C4793}"/>
   </bookViews>
@@ -47,338 +47,304 @@
         <r>
           <rPr>
             <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[클래스 ID]</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+101 : 전사(남)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+102 : 버서커
+103 : 디스트로이어,
+104 : 워로드
+105 : 홀리나이트
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>111 : 전사 (여)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+112 : 슬레이어
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>201 : 마법사</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+202 : 아르카나
+203 : 서머너
+204 : 바드
+205 : 소서리스
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>301 : 무도가 (여)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+302 : 배틀마스터
+303 : 인파이터
+304 : 기공사
+305 : 창술사 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>311 : 무도가 (남)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+312 : 스트라이커
+313 : 브레이커
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>401 : 암살자</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+402 : 블레이드
+403 : 데모닉
+404 : 리퍼
+405 : 소울이터 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>501 : 헌터 (남)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+502 : 데빌헌터
+503 : 호크아이
+504 : 블래스터
+505 : 스카우터
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>511 : 헌터 (여)</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+512 : 건슬링어
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>601 : 스페셜리스트</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="맑은 고딕"/>
+            <family val="3"/>
+            <charset val="129"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+602 : 도화가
+603 : 기상술사
+604 : 환수사</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F8" authorId="0" shapeId="0" xr:uid="{2B369155-C557-42B7-BF94-4F1DF83919E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t>클래스</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          <t>[스킬 종류]</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve"> ID
-101 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>전사</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>(</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>남</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-102 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>버서커</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-103 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>디스트로이어</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">,
-104 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>워로드</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-105 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">홀리나이트
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">111 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>전사</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>여</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-112 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">슬레이어
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">201 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>마법사</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
           <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">202 : </t>
-        </r>
-        <r>
-          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t xml:space="preserve">아르카나
+          <t xml:space="preserve">0 : 기본 공격(평타)
+1 : 이동기
+2 : 기상기
 </t>
         </r>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">203 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">서머너
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">204 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">바드
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">205 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>소서리스</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -388,256 +354,35 @@
             <b/>
             <sz val="9"/>
             <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">301 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t>무도가</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
+          <t>10 : 일반 스킬</t>
+        </r>
+        <r>
+          <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t>여</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">
-302 : </t>
-        </r>
-        <r>
-          <rPr>
+11 : 일반 스킬 세부 분류 1 (ex: 창술사 - 난무 스킬)
+12 : 일반 스킬 세부 분류 2 (ex: 창술사 - 집중 스킬)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t xml:space="preserve">배틀마스터
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">303 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">인파이터
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">304 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">기공사
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">305 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>창술사</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> 
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">311 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>무도가</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>남</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-312 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">스트라이커
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">313 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">브레이커
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">401 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>암살자</t>
+          <t>20 : 아이덴티티 스킬</t>
         </r>
         <r>
           <rPr>
@@ -652,408 +397,14 @@
         </r>
         <r>
           <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">402 : </t>
-        </r>
-        <r>
-          <rPr>
+            <b/>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="돋움"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t xml:space="preserve">블레이드
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">403 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">데모닉
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">404 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">리퍼
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">405 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>소울이터</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">501 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>헌터</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>남</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-502 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">데빌헌터
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">503 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">호크아이
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">504 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">블래스터
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">505 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>스카우터</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">511 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>헌터</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> (</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>여</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>)</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-512 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">건슬링어
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">601 : </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>스페셜리스트</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">602 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">도화가
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">603 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t xml:space="preserve">기상술사
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">604 : </t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
-            <family val="3"/>
-            <charset val="129"/>
-          </rPr>
-          <t>환수사</t>
+          <t>30 : 각성기</t>
         </r>
       </text>
     </comment>
@@ -1786,33 +1137,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (Skill_String_Table.xlsx의 id)</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>스킬 종류</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-0 : 기본 공격 / 1: 일반 스킬 / 2: 아이덴티티 스킬 / 3: 각성기 / 4: 이동기 / 5: 기상기</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2138,6 +1462,36 @@
     <t>OOO/OO/O -&gt; 클래스id/번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">'고유의 특징'에 따라 분류되는 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">스킬 종류
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0 : 기본 공격 / 1: 일반 스킬 / 2: 아이덴티티 스킬 / 3: 각성기 / 4: 이동기 / 5: 기상기</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -2148,7 +1502,7 @@
     <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="178" formatCode="00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2255,35 +1609,60 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <color rgb="FF0070C0"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="4"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF00B050"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF0070C0"/>
+      <color indexed="81"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -2738,27 +2117,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2792,7 +2150,28 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3115,27 +2494,29 @@
   <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="4.3984375" style="37" customWidth="1"/>
+    <col min="1" max="1" width="8.796875" style="3"/>
+    <col min="2" max="2" width="4.3984375" style="13" customWidth="1"/>
     <col min="3" max="3" width="4.3984375" style="13" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="18.09765625" style="2" customWidth="1"/>
     <col min="6" max="6" width="75.3984375" style="2" customWidth="1"/>
-    <col min="7" max="9" width="8.69921875" customWidth="1"/>
+    <col min="7" max="9" width="8.69921875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.796875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:11" ht="18" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="35"/>
-      <c r="E2" s="36"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="51"/>
       <c r="H2" s="52" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" s="52"/>
       <c r="J2" s="52"/>
@@ -3156,7 +2537,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="52" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="52"/>
       <c r="J3" s="52"/>
@@ -3177,26 +2558,26 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I4" s="53"/>
       <c r="J4" s="53"/>
       <c r="K4" s="53"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="34">
         <v>1</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="37" t="s">
         <v>44</v>
       </c>
       <c r="G5" s="4"/>
@@ -3206,19 +2587,19 @@
       <c r="K5" s="53"/>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="38">
         <v>2</v>
       </c>
-      <c r="D6" s="46" t="s">
+      <c r="D6" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="41" t="s">
         <v>48</v>
       </c>
       <c r="G6" s="4"/>
@@ -3228,20 +2609,20 @@
       <c r="K6" s="53"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B7" s="39" t="s">
+      <c r="B7" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="45">
+      <c r="C7" s="38">
         <v>3</v>
       </c>
-      <c r="D7" s="46" t="s">
+      <c r="D7" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="47" t="s">
+      <c r="E7" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="48" t="s">
-        <v>51</v>
+      <c r="F7" s="41" t="s">
+        <v>50</v>
       </c>
       <c r="H7" s="53"/>
       <c r="I7" s="53"/>
@@ -3256,8 +2637,8 @@
       <c r="E8" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="17" t="s">
-        <v>49</v>
+      <c r="F8" s="45" t="s">
+        <v>57</v>
       </c>
       <c r="H8" s="53"/>
       <c r="I8" s="53"/>
@@ -3273,7 +2654,7 @@
         <v>43</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" s="53"/>
       <c r="I9" s="53"/>
@@ -3289,7 +2670,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H10" s="53"/>
       <c r="I10" s="53"/>
@@ -3327,7 +2708,7 @@
       <c r="K13" s="53"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.4">
-      <c r="B14" s="40"/>
+      <c r="B14" s="48"/>
       <c r="C14" s="14"/>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
@@ -3348,16 +2729,16 @@
       <c r="K15" s="53"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F18" s="50"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F19" s="51" t="s">
-        <v>55</v>
+      <c r="F19" s="44" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.4">
-      <c r="F20" s="51" t="s">
-        <v>56</v>
+      <c r="F20" s="44" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -4004,7 +3385,7 @@
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B18" s="49"/>
+      <c r="B18" s="42"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>